<commit_message>
Add choose input table
</commit_message>
<xml_diff>
--- a/Documents/ImportData.xlsx
+++ b/Documents/ImportData.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>D0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>D1</t>
   </si>
@@ -52,9 +49,6 @@
   </si>
   <si>
     <t>T5</t>
-  </si>
-  <si>
-    <t>D7</t>
   </si>
 </sst>
 </file>
@@ -86,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,30 +103,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -436,43 +416,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>615</v>
@@ -492,13 +467,10 @@
       <c r="G2" s="2">
         <v>65</v>
       </c>
-      <c r="H2" s="2">
-        <v>65</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>15</v>
@@ -518,13 +490,10 @@
       <c r="G3" s="2">
         <v>816</v>
       </c>
-      <c r="H3" s="2">
-        <v>816</v>
-      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -544,13 +513,10 @@
       <c r="G4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>312</v>
@@ -570,13 +536,10 @@
       <c r="G5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="2">
-        <v>2</v>
-      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>45</v>
@@ -594,9 +557,6 @@
         <v>491</v>
       </c>
       <c r="G6" s="2">
-        <v>59</v>
-      </c>
-      <c r="H6" s="2">
         <v>59</v>
       </c>
     </row>

</xml_diff>